<commit_message>
add 3 level categories relationship and design database
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
@@ -14,44 +14,26 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
   <si>
     <t>Date</t>
   </si>
   <si>
-    <t>Type</t>
-  </si>
-  <si>
     <t>Works List</t>
   </si>
   <si>
-    <t>Order rest service</t>
-  </si>
-  <si>
     <t>8300,8301,8302,……</t>
   </si>
   <si>
     <t>Ports</t>
   </si>
   <si>
-    <t>Create Order</t>
-  </si>
-  <si>
-    <t>Fetch Order</t>
-  </si>
-  <si>
-    <t>Delete Order</t>
-  </si>
-  <si>
     <t>Database</t>
   </si>
   <si>
     <t>NoSQL(MongoDB)</t>
   </si>
   <si>
-    <t>Product rest service</t>
-  </si>
-  <si>
     <t>8200,8201,8202,…….</t>
   </si>
   <si>
@@ -59,13 +41,40 @@
   </si>
   <si>
     <t>Admin UI service</t>
+  </si>
+  <si>
+    <t>8100,8101,8102,….</t>
+  </si>
+  <si>
+    <t>MySQL Database</t>
+  </si>
+  <si>
+    <t>Server</t>
+  </si>
+  <si>
+    <t>Tomcate Server</t>
+  </si>
+  <si>
+    <t>Apache Server</t>
+  </si>
+  <si>
+    <t>Service Name</t>
+  </si>
+  <si>
+    <t>Category Rest Service</t>
+  </si>
+  <si>
+    <t>Order Rest service</t>
+  </si>
+  <si>
+    <t>Product Rest service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -85,8 +94,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -96,6 +111,30 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0099FF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -112,17 +151,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -131,6 +187,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF0099FF"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -145,7 +206,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Blue Warm">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -153,34 +214,34 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="242852"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="ACCBF9"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="4A66AC"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="629DD1"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="297FD5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="7F8FA9"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="5AA2AE"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="9D90A0"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="9454C3"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="3EBBF0"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
@@ -429,95 +490,189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:F13"/>
+  <dimension ref="A3:H15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.140625" style="1"/>
-    <col min="2" max="2" width="18" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="31" style="1" customWidth="1"/>
-    <col min="4" max="4" width="23.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="75" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" style="1" customWidth="1"/>
-    <col min="7" max="16384" width="9.140625" style="1"/>
+    <col min="4" max="4" width="34.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="26.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="29.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="23.7109375" style="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
       <c r="A3" s="2"/>
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A7" s="5"/>
+      <c r="B7" s="6">
+        <v>44260</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
+      <c r="G7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="5"/>
+    </row>
+    <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="4"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4"/>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8">
+        <v>44262</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E10" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="H10" s="7"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+    </row>
+    <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="11">
+        <v>44263</v>
+      </c>
+      <c r="C12" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="12">
+        <v>8080</v>
+      </c>
+      <c r="E12" s="10"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="H12" s="10"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A13" s="4"/>
+      <c r="B13" s="4"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="4"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A14" s="13"/>
+      <c r="B14" s="14">
+        <v>44266</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
-        <v>44260</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="1" t="s">
+      <c r="E14" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="13" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E8" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="E9" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B11" s="4">
-        <v>44262</v>
-      </c>
-      <c r="C11" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E11" s="1" t="s">
+      <c r="G14" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="4">
-        <v>44263</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="5">
-        <v>8080</v>
-      </c>
+      <c r="H14" s="13"/>
+    </row>
+    <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A15" s="4"/>
+      <c r="B15" s="4"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
service registry module add
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Date</t>
   </si>
@@ -68,6 +68,9 @@
   </si>
   <si>
     <t>Product Rest service</t>
+  </si>
+  <si>
+    <t>Service Registry</t>
   </si>
 </sst>
 </file>
@@ -101,18 +104,12 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -138,6 +135,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDCCA5E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -151,34 +160,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -189,6 +206,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFDCCA5E"/>
       <color rgb="FF0099FF"/>
     </mruColors>
   </colors>
@@ -490,10 +508,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H15"/>
+  <dimension ref="A3:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="A3" sqref="A3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -509,170 +527,186 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="A3" s="17"/>
+      <c r="B3" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="3"/>
+      <c r="H3" s="18"/>
     </row>
     <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6">
+      <c r="A7" s="3"/>
+      <c r="B7" s="4">
         <v>44260</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G7" s="5" t="s">
+      <c r="G7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="5"/>
+      <c r="H7" s="3"/>
     </row>
     <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
     </row>
     <row r="9" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="7"/>
-      <c r="B10" s="8">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6">
         <v>44262</v>
       </c>
-      <c r="C10" s="9" t="s">
+      <c r="C10" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="D10" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="7" t="s">
+      <c r="F10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="7" t="s">
+      <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="7"/>
+      <c r="H10" s="5"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="11">
+      <c r="A12" s="8"/>
+      <c r="B12" s="9">
         <v>44263</v>
       </c>
-      <c r="C12" s="10" t="s">
+      <c r="C12" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D12" s="12">
+      <c r="D12" s="10">
         <v>8080</v>
       </c>
-      <c r="E12" s="10"/>
-      <c r="F12" s="10"/>
-      <c r="G12" s="10" t="s">
+      <c r="E12" s="8"/>
+      <c r="F12" s="8"/>
+      <c r="G12" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="H12" s="10"/>
+      <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
     </row>
     <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="13"/>
-      <c r="B14" s="14">
+      <c r="A14" s="11"/>
+      <c r="B14" s="12">
         <v>44266</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="13" t="s">
+      <c r="D14" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F14" s="13" t="s">
+      <c r="F14" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G14" s="13" t="s">
+      <c r="G14" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="H14" s="13"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A17" s="13"/>
+      <c r="B17" s="14">
+        <v>44271</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="16">
+        <v>8761</v>
+      </c>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
initial commit from version 2
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
   <si>
     <t>Date</t>
   </si>
@@ -71,13 +71,34 @@
   </si>
   <si>
     <t>Service Registry</t>
+  </si>
+  <si>
+    <t>Some Useful Resources</t>
+  </si>
+  <si>
+    <t>http://www.myspsolution.com/news-events/rest-vs-messaging-for-microservices-which-one-is-best/</t>
+  </si>
+  <si>
+    <t>https://blog.logrocket.com/methods-for-microservice-communication/</t>
+  </si>
+  <si>
+    <t>https://reflectoring.io/event-messaging-with-spring-boot-and-rabbitmq/</t>
+  </si>
+  <si>
+    <t>******</t>
+  </si>
+  <si>
+    <t>***</t>
+  </si>
+  <si>
+    <t>https://medium.com/@sopheamak/rabbitqm-with-springboot-fd085dcab484</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,8 +124,15 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="2" tint="-0.249977111117893"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,6 +172,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFDCCA5E"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -160,7 +194,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -198,6 +232,8 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +544,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H17"/>
+  <dimension ref="A3:H50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,6 +744,38 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
+    <row r="45" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B45" s="19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C45" s="20"/>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add resources to the work-flow sheet
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>Date</t>
   </si>
@@ -92,6 +92,12 @@
   </si>
   <si>
     <t>https://medium.com/@sopheamak/rabbitqm-with-springboot-fd085dcab484</t>
+  </si>
+  <si>
+    <t>https://www.devglan.com/spring-boot/springboot-rabbitmq-example</t>
+  </si>
+  <si>
+    <t>https://www.petermorlion.com/rabbitmq-use-cases/</t>
   </si>
 </sst>
 </file>
@@ -544,10 +550,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H50"/>
+  <dimension ref="A3:H54"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+      <selection activeCell="B54" sqref="B54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -776,6 +782,19 @@
         <v>25</v>
       </c>
     </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add rabbitAMQ and Configure it and also added hystrix fault tollerance
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Date</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>https://www.petermorlion.com/rabbitmq-use-cases/</t>
+  </si>
+  <si>
+    <t>https://medium.com/swlh/make-your-microservices-bulletproof-with-netflix-hystrix-853c1c308f08</t>
   </si>
 </sst>
 </file>
@@ -550,10 +553,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H54"/>
+  <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B54" sqref="B54"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -795,6 +798,11 @@
         <v>27</v>
       </c>
     </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fixing some categories issues
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Date</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>https://medium.com/swlh/make-your-microservices-bulletproof-with-netflix-hystrix-853c1c308f08</t>
+  </si>
+  <si>
+    <t>API gateway</t>
   </si>
 </sst>
 </file>
@@ -203,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -243,6 +246,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -555,8 +561,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="B55" sqref="B55"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,6 +759,17 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="21">
+        <v>44290</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="1">
+        <v>9090</v>
+      </c>
+    </row>
     <row r="45" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B45" s="19" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
registering services with eureka server
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -206,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -247,6 +247,9 @@
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -561,7 +564,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
@@ -766,7 +769,7 @@
       <c r="C21" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="22">
         <v>9090</v>
       </c>
     </row>

</xml_diff>

<commit_message>
customer rest endpoints create
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
     <t>Date</t>
   </si>
@@ -104,13 +104,16 @@
   </si>
   <si>
     <t>API gateway</t>
+  </si>
+  <si>
+    <t>Customer Service</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -143,8 +146,14 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +199,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +227,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -246,10 +267,14 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -565,7 +590,7 @@
   <dimension ref="A3:H55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A24" sqref="A24:H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -762,16 +787,35 @@
       <c r="G17" s="13"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="21">
+    <row r="21" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A21" s="21"/>
+      <c r="B21" s="22">
         <v>44290</v>
       </c>
-      <c r="C21" s="1" t="s">
+      <c r="C21" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="D21" s="22">
+      <c r="D21" s="23">
         <v>9090</v>
       </c>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="21"/>
+      <c r="H21" s="21"/>
+    </row>
+    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A24" s="24"/>
+      <c r="B24" s="24"/>
+      <c r="C24" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="24">
+        <v>9292</v>
+      </c>
+      <c r="E24" s="24"/>
+      <c r="F24" s="24"/>
+      <c r="G24" s="24"/>
+      <c r="H24" s="24"/>
     </row>
     <row r="45" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
       <c r="B45" s="19" t="s">

</xml_diff>

<commit_message>
fetching issues may be resolved
</commit_message>
<xml_diff>
--- a/work-flow.xlsx
+++ b/work-flow.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Date</t>
   </si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Customer Service</t>
+  </si>
+  <si>
+    <t>20/06/2021</t>
+  </si>
+  <si>
+    <t>Payment Servcie</t>
   </si>
 </sst>
 </file>
@@ -153,7 +159,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -211,6 +217,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -227,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,7 +265,6 @@
     <xf numFmtId="14" fontId="3" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="14" fontId="3" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -275,6 +286,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -589,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A24" sqref="A24:H24"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,64 +623,57 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:8" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18" t="s">
+      <c r="A3" s="16"/>
+      <c r="B3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="18" t="s">
+      <c r="C3" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="18" t="s">
+      <c r="D3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="E3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="18" t="s">
+      <c r="F3" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="18"/>
+      <c r="H3" s="17"/>
     </row>
     <row r="6" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="B6" s="13">
+        <v>44271</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="15">
+        <v>8761</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
     </row>
     <row r="7" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4">
-        <v>44260</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H7" s="3"/>
+      <c r="A7" s="2"/>
     </row>
     <row r="8" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
+      <c r="B8" s="21">
+        <v>44290</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="22">
+        <v>9090</v>
+      </c>
       <c r="E8" s="2"/>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
@@ -680,7 +690,6 @@
       <c r="H9" s="2"/>
     </row>
     <row r="10" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
       <c r="B10" s="6">
         <v>44262</v>
       </c>
@@ -699,7 +708,7 @@
       <c r="G10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="H10" s="5"/>
+      <c r="H10" s="2"/>
     </row>
     <row r="11" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A11" s="2"/>
@@ -712,22 +721,25 @@
       <c r="H11" s="2"/>
     </row>
     <row r="12" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A12" s="8"/>
-      <c r="B12" s="9">
-        <v>44263</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D12" s="10">
-        <v>8080</v>
-      </c>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="8"/>
+      <c r="B12" s="12">
+        <v>44266</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="F12" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="2"/>
     </row>
     <row r="13" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
       <c r="A13" s="2"/>
@@ -737,96 +749,91 @@
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-    </row>
-    <row r="14" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A14" s="11"/>
-      <c r="B14" s="12">
-        <v>44266</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F14" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="H14" s="11"/>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B14" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="23">
+        <v>9292</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
       <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-    </row>
-    <row r="17" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14">
-        <v>44271</v>
-      </c>
-      <c r="C17" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="16">
-        <v>8761</v>
-      </c>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
-    </row>
-    <row r="21" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22">
-        <v>44290</v>
-      </c>
-      <c r="C21" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="D21" s="23">
-        <v>9090</v>
-      </c>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-    </row>
-    <row r="24" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="24"/>
-      <c r="B24" s="24"/>
-      <c r="C24" s="24" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="24">
-        <v>9292</v>
-      </c>
-      <c r="E24" s="24"/>
-      <c r="F24" s="24"/>
-      <c r="G24" s="24"/>
-      <c r="H24" s="24"/>
+    </row>
+    <row r="16" spans="1:8" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B16" s="9">
+        <v>44263</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="10">
+        <v>8080</v>
+      </c>
+      <c r="E16" s="9"/>
+      <c r="F16" s="8"/>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="18" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B18" s="4">
+        <v>44260</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="B20" s="25">
+        <v>44373</v>
+      </c>
+      <c r="C20" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="D20" s="24">
+        <v>9393</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="45" spans="1:3" ht="20.25" x14ac:dyDescent="0.3">
-      <c r="B45" s="19" t="s">
+      <c r="A45" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B45" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="20"/>
+      <c r="C45" s="19"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>24</v>
-      </c>
       <c r="B46" s="1" t="s">
         <v>20</v>
       </c>
@@ -836,33 +843,27 @@
         <v>21</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B49" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B50" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="1" t="s">
-        <v>23</v>
-      </c>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B52" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B54" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B55" s="1" t="s">
         <v>28</v>
       </c>

</xml_diff>